<commit_message>
agrego autores a metodologia
</commit_message>
<xml_diff>
--- a/analisis/resultados/argentina/metadata_arg.xlsx
+++ b/analisis/resultados/argentina/metadata_arg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos\repos\hidrocarburos\analisis\resultados\argentina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9B56D5-0734-4E84-BEF8-6402BA7438D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9310E781-F9E7-478A-BDE4-813BF88F7D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1366,7 +1366,7 @@
   <dimension ref="A1:D161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="B157" sqref="B157"/>
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,41 +1406,41 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>226</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>166</v>
       </c>
       <c r="D5" t="s">
         <v>169</v>
@@ -1448,141 +1448,153 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
-        <v>202</v>
+        <v>197</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>169</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>199</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>182</v>
+        <v>185</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>237</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>182</v>
+        <v>186</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>280</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>220</v>
       </c>
       <c r="D16" t="s">
         <v>169</v>
@@ -1590,69 +1602,69 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>183</v>
+        <v>279</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>220</v>
       </c>
       <c r="D17" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>134</v>
       </c>
       <c r="B18" t="s">
-        <v>183</v>
+        <v>298</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>222</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="B19" t="s">
-        <v>183</v>
+        <v>286</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>220</v>
       </c>
       <c r="D19" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>157</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>313</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>227</v>
       </c>
       <c r="D20" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>158</v>
       </c>
       <c r="B21" t="s">
-        <v>184</v>
+        <v>318</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>227</v>
       </c>
       <c r="D21" t="s">
         <v>169</v>
@@ -1660,139 +1672,136 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
-        <v>184</v>
+        <v>229</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>184</v>
+        <v>287</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>220</v>
       </c>
       <c r="D24" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>122</v>
       </c>
       <c r="B25" t="s">
-        <v>184</v>
+        <v>284</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>220</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>184</v>
-      </c>
-      <c r="C26" t="s">
-        <v>12</v>
+        <v>202</v>
       </c>
       <c r="D26" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>139</v>
       </c>
       <c r="B28" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>166</v>
       </c>
       <c r="D28" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
-        <v>187</v>
+        <v>258</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="D31" t="s">
         <v>169</v>
@@ -1800,24 +1809,24 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>203</v>
+        <v>266</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
       <c r="D32" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C33" t="s">
         <v>35</v>
@@ -1828,7 +1837,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
         <v>205</v>
@@ -1837,12 +1846,12 @@
         <v>35</v>
       </c>
       <c r="D34" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
         <v>205</v>
@@ -1851,21 +1860,21 @@
         <v>35</v>
       </c>
       <c r="D35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="C36" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1884,587 +1893,581 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="C40" t="s">
         <v>35</v>
       </c>
       <c r="D40" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B41" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="C41" t="s">
         <v>35</v>
       </c>
       <c r="D41" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C42" t="s">
         <v>35</v>
       </c>
       <c r="D42" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B43" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C43" t="s">
         <v>35</v>
       </c>
       <c r="D43" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>127</v>
       </c>
       <c r="B44" t="s">
-        <v>209</v>
+        <v>291</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>166</v>
       </c>
       <c r="D44" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B45" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="C45" t="s">
-        <v>35</v>
+        <v>221</v>
       </c>
       <c r="D45" t="s">
-        <v>175</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
-        <v>195</v>
+        <v>273</v>
       </c>
       <c r="C46" t="s">
-        <v>35</v>
+        <v>220</v>
       </c>
       <c r="D46" t="s">
-        <v>175</v>
+        <v>271</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="B47" t="s">
-        <v>196</v>
+        <v>272</v>
       </c>
       <c r="C47" t="s">
-        <v>35</v>
+        <v>220</v>
       </c>
       <c r="D47" t="s">
-        <v>175</v>
+        <v>271</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>136</v>
       </c>
       <c r="B48" t="s">
-        <v>197</v>
+        <v>230</v>
       </c>
       <c r="C48" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D48" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>141</v>
       </c>
       <c r="B49" t="s">
-        <v>198</v>
+        <v>299</v>
       </c>
       <c r="C49" t="s">
-        <v>35</v>
+        <v>220</v>
       </c>
       <c r="D49" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="B50" t="s">
-        <v>211</v>
+        <v>303</v>
       </c>
       <c r="C50" t="s">
-        <v>35</v>
+        <v>220</v>
       </c>
       <c r="D50" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>131</v>
       </c>
       <c r="B51" t="s">
-        <v>212</v>
+        <v>295</v>
       </c>
       <c r="C51" t="s">
-        <v>35</v>
+        <v>220</v>
       </c>
       <c r="D51" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>213</v>
-      </c>
-      <c r="C52" t="s">
-        <v>35</v>
+        <v>182</v>
       </c>
       <c r="D52" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="C53" t="s">
-        <v>35</v>
+        <v>232</v>
       </c>
       <c r="D53" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B54" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
       <c r="C54" t="s">
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="D54" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B55" t="s">
-        <v>199</v>
+        <v>246</v>
       </c>
       <c r="C55" t="s">
-        <v>35</v>
+        <v>233</v>
       </c>
       <c r="D55" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="B56" t="s">
-        <v>200</v>
+        <v>270</v>
       </c>
       <c r="C56" t="s">
-        <v>35</v>
+        <v>220</v>
       </c>
       <c r="D56" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C57" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>196</v>
-      </c>
-      <c r="C58" t="s">
-        <v>35</v>
+        <v>182</v>
       </c>
       <c r="D58" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="B59" t="s">
-        <v>215</v>
+        <v>289</v>
       </c>
       <c r="C59" t="s">
-        <v>35</v>
+        <v>220</v>
       </c>
       <c r="D59" t="s">
-        <v>216</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="B60" t="s">
-        <v>217</v>
+        <v>281</v>
       </c>
       <c r="C60" t="s">
-        <v>35</v>
+        <v>220</v>
       </c>
       <c r="D60" t="s">
-        <v>216</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B61" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="C61" t="s">
-        <v>35</v>
+        <v>221</v>
       </c>
       <c r="D61" t="s">
-        <v>179</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="B62" t="s">
-        <v>215</v>
+        <v>292</v>
       </c>
       <c r="C62" t="s">
-        <v>35</v>
+        <v>220</v>
       </c>
       <c r="D62" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>159</v>
       </c>
       <c r="B63" t="s">
-        <v>219</v>
+        <v>316</v>
       </c>
       <c r="C63" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D63" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>160</v>
       </c>
       <c r="B64" t="s">
-        <v>219</v>
+        <v>317</v>
       </c>
       <c r="C64" t="s">
         <v>35</v>
       </c>
       <c r="D64" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>219</v>
+        <v>182</v>
       </c>
       <c r="C65" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D65" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C66" t="s">
         <v>35</v>
       </c>
       <c r="D66" t="s">
-        <v>171</v>
+        <v>216</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C67" t="s">
         <v>35</v>
       </c>
       <c r="D67" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="B68" t="s">
-        <v>219</v>
+        <v>184</v>
       </c>
       <c r="C68" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D68" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="B69" t="s">
-        <v>235</v>
+        <v>184</v>
       </c>
       <c r="C69" t="s">
-        <v>236</v>
+        <v>12</v>
       </c>
       <c r="D69" t="s">
-        <v>238</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>235</v>
+        <v>184</v>
       </c>
       <c r="C70" t="s">
-        <v>236</v>
+        <v>12</v>
       </c>
       <c r="D70" t="s">
-        <v>239</v>
+        <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="C71" t="s">
-        <v>221</v>
+        <v>35</v>
       </c>
       <c r="D71" t="s">
-        <v>241</v>
+        <v>179</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="C72" t="s">
-        <v>221</v>
+        <v>35</v>
       </c>
       <c r="D72" t="s">
-        <v>241</v>
+        <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B73" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="C73" t="s">
-        <v>231</v>
+        <v>35</v>
       </c>
       <c r="D73" t="s">
-        <v>241</v>
+        <v>178</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B74" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
       <c r="C74" t="s">
-        <v>231</v>
+        <v>35</v>
       </c>
       <c r="D74" t="s">
-        <v>241</v>
+        <v>171</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B75" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="C75" t="s">
-        <v>222</v>
+        <v>35</v>
       </c>
       <c r="D75" t="s">
-        <v>241</v>
+        <v>170</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="B76" t="s">
-        <v>246</v>
+        <v>184</v>
       </c>
       <c r="C76" t="s">
-        <v>232</v>
+        <v>12</v>
       </c>
       <c r="D76" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="B77" t="s">
-        <v>246</v>
+        <v>184</v>
       </c>
       <c r="C77" t="s">
-        <v>233</v>
+        <v>12</v>
       </c>
       <c r="D77" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B78" t="s">
-        <v>246</v>
+        <v>219</v>
       </c>
       <c r="C78" t="s">
-        <v>234</v>
+        <v>35</v>
       </c>
       <c r="D78" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B79" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="C79" t="s">
-        <v>220</v>
+        <v>12</v>
       </c>
       <c r="D79" t="s">
         <v>169</v>
@@ -2472,13 +2475,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="B80" t="s">
-        <v>248</v>
+        <v>206</v>
       </c>
       <c r="C80" t="s">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="D80" t="s">
         <v>169</v>
@@ -2486,55 +2489,55 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="B81" t="s">
-        <v>250</v>
+        <v>204</v>
       </c>
       <c r="C81" t="s">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="D81" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="B82" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
       <c r="C82" t="s">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="D82" t="s">
-        <v>251</v>
+        <v>179</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B83" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
       <c r="C83" t="s">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="D83" t="s">
-        <v>169</v>
+        <v>237</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B84" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="C84" t="s">
-        <v>220</v>
+        <v>12</v>
       </c>
       <c r="D84" t="s">
         <v>169</v>
@@ -2542,27 +2545,27 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B85" t="s">
-        <v>235</v>
+        <v>264</v>
       </c>
       <c r="C85" t="s">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="D85" t="s">
-        <v>238</v>
+        <v>169</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>254</v>
+        <v>21</v>
       </c>
       <c r="B86" t="s">
-        <v>255</v>
+        <v>184</v>
       </c>
       <c r="C86" t="s">
-        <v>220</v>
+        <v>12</v>
       </c>
       <c r="D86" t="s">
         <v>169</v>
@@ -2570,38 +2573,41 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>161</v>
       </c>
       <c r="B87" t="s">
-        <v>256</v>
+        <v>315</v>
       </c>
       <c r="C87" t="s">
-        <v>220</v>
+        <v>12</v>
+      </c>
+      <c r="D87" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>155</v>
       </c>
       <c r="B88" t="s">
-        <v>257</v>
+        <v>311</v>
       </c>
       <c r="C88" t="s">
-        <v>166</v>
+        <v>12</v>
       </c>
       <c r="D88" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>162</v>
       </c>
       <c r="B89" t="s">
-        <v>258</v>
+        <v>314</v>
       </c>
       <c r="C89" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D89" t="s">
         <v>169</v>
@@ -2609,10 +2615,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>3</v>
       </c>
       <c r="B90" t="s">
-        <v>259</v>
+        <v>181</v>
       </c>
       <c r="C90" t="s">
         <v>4</v>
@@ -2623,27 +2629,27 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="B91" t="s">
-        <v>260</v>
+        <v>203</v>
       </c>
       <c r="C91" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="D91" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C92" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D92" t="s">
         <v>169</v>
@@ -2651,13 +2657,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>152</v>
       </c>
       <c r="B93" t="s">
-        <v>262</v>
+        <v>308</v>
       </c>
       <c r="C93" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D93" t="s">
         <v>169</v>
@@ -2665,27 +2671,27 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>95</v>
+        <v>153</v>
       </c>
       <c r="B94" t="s">
-        <v>263</v>
+        <v>309</v>
       </c>
       <c r="C94" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="D94" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>154</v>
       </c>
       <c r="B95" t="s">
-        <v>247</v>
+        <v>310</v>
       </c>
       <c r="C95" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D95" t="s">
         <v>169</v>
@@ -2693,24 +2699,24 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B96" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C96" t="s">
-        <v>35</v>
+        <v>166</v>
       </c>
       <c r="D96" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="B97" t="s">
-        <v>248</v>
+        <v>285</v>
       </c>
       <c r="C97" t="s">
         <v>220</v>
@@ -2721,41 +2727,41 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>265</v>
+        <v>202</v>
       </c>
       <c r="C98" t="s">
-        <v>166</v>
+        <v>4</v>
       </c>
       <c r="D98" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B99" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="C99" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D99" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="B100" t="s">
-        <v>252</v>
+        <v>305</v>
       </c>
       <c r="C100" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D100" t="s">
         <v>169</v>
@@ -2763,10 +2769,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="B101" t="s">
-        <v>253</v>
+        <v>305</v>
       </c>
       <c r="C101" t="s">
         <v>220</v>
@@ -2777,66 +2783,66 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>103</v>
+        <v>148</v>
       </c>
       <c r="B102" t="s">
-        <v>267</v>
+        <v>306</v>
       </c>
       <c r="C102" t="s">
-        <v>166</v>
+        <v>221</v>
       </c>
       <c r="D102" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="B103" t="s">
-        <v>249</v>
+        <v>306</v>
       </c>
       <c r="C103" t="s">
         <v>220</v>
       </c>
       <c r="D103" t="s">
-        <v>251</v>
+        <v>169</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B104" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C104" t="s">
-        <v>4</v>
+        <v>220</v>
       </c>
       <c r="D104" t="s">
-        <v>269</v>
+        <v>169</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B105" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C105" t="s">
         <v>220</v>
       </c>
       <c r="D105" t="s">
-        <v>268</v>
+        <v>169</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="B106" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="C106" t="s">
         <v>220</v>
@@ -2847,30 +2853,30 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="B107" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="C107" t="s">
         <v>220</v>
       </c>
       <c r="D107" t="s">
-        <v>271</v>
+        <v>169</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>109</v>
+        <v>254</v>
       </c>
       <c r="B108" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="C108" t="s">
         <v>220</v>
       </c>
       <c r="D108" t="s">
-        <v>271</v>
+        <v>169</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2889,66 +2895,66 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="B110" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="C110" t="s">
-        <v>166</v>
+        <v>220</v>
       </c>
       <c r="D110" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="B111" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
       <c r="C111" t="s">
-        <v>166</v>
+        <v>220</v>
       </c>
       <c r="D111" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B112" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="C112" t="s">
-        <v>166</v>
+        <v>222</v>
       </c>
       <c r="D112" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="B113" t="s">
-        <v>278</v>
+        <v>296</v>
       </c>
       <c r="C113" t="s">
-        <v>166</v>
+        <v>222</v>
       </c>
       <c r="D113" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B114" t="s">
-        <v>279</v>
+        <v>252</v>
       </c>
       <c r="C114" t="s">
         <v>220</v>
@@ -2959,10 +2965,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B115" t="s">
-        <v>280</v>
+        <v>253</v>
       </c>
       <c r="C115" t="s">
         <v>220</v>
@@ -2973,83 +2979,80 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="B116" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="C116" t="s">
         <v>220</v>
       </c>
-      <c r="D116" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="B117" t="s">
-        <v>289</v>
+        <v>249</v>
       </c>
       <c r="C117" t="s">
         <v>220</v>
       </c>
       <c r="D117" t="s">
-        <v>169</v>
+        <v>251</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B118" t="s">
-        <v>286</v>
+        <v>249</v>
       </c>
       <c r="C118" t="s">
-        <v>220</v>
+        <v>4</v>
       </c>
       <c r="D118" t="s">
-        <v>169</v>
+        <v>269</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B119" t="s">
-        <v>282</v>
+        <v>249</v>
       </c>
       <c r="C119" t="s">
         <v>220</v>
       </c>
       <c r="D119" t="s">
-        <v>169</v>
+        <v>251</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B120" t="s">
-        <v>283</v>
+        <v>249</v>
       </c>
       <c r="C120" t="s">
         <v>220</v>
       </c>
       <c r="D120" t="s">
-        <v>169</v>
+        <v>268</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="B121" t="s">
-        <v>284</v>
+        <v>224</v>
       </c>
       <c r="C121" t="s">
-        <v>220</v>
+        <v>166</v>
       </c>
       <c r="D121" t="s">
         <v>169</v>
@@ -3057,108 +3060,108 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>123</v>
+        <v>7</v>
       </c>
       <c r="B122" t="s">
-        <v>285</v>
+        <v>202</v>
       </c>
       <c r="C122" t="s">
-        <v>220</v>
+        <v>4</v>
       </c>
       <c r="D122" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>124</v>
+        <v>77</v>
       </c>
       <c r="B123" t="s">
-        <v>288</v>
+        <v>245</v>
       </c>
       <c r="C123" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D123" t="s">
-        <v>169</v>
+        <v>241</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="B124" t="s">
-        <v>287</v>
+        <v>235</v>
       </c>
       <c r="C124" t="s">
         <v>220</v>
       </c>
       <c r="D124" t="s">
-        <v>169</v>
+        <v>238</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="B125" t="s">
-        <v>290</v>
+        <v>235</v>
       </c>
       <c r="C125" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="D125" t="s">
-        <v>169</v>
+        <v>239</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>127</v>
+        <v>71</v>
       </c>
       <c r="B126" t="s">
-        <v>291</v>
+        <v>235</v>
       </c>
       <c r="C126" t="s">
-        <v>166</v>
+        <v>236</v>
       </c>
       <c r="D126" t="s">
-        <v>169</v>
+        <v>238</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>128</v>
+        <v>75</v>
       </c>
       <c r="B127" t="s">
-        <v>292</v>
+        <v>243</v>
       </c>
       <c r="C127" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="D127" t="s">
-        <v>169</v>
+        <v>241</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>129</v>
+        <v>76</v>
       </c>
       <c r="B128" t="s">
-        <v>293</v>
+        <v>244</v>
       </c>
       <c r="C128" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="D128" t="s">
-        <v>169</v>
+        <v>241</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="B129" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="C129" t="s">
         <v>222</v>
@@ -3169,13 +3172,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="B130" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="C130" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D130" t="s">
         <v>169</v>
@@ -3183,10 +3186,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="B131" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="C131" t="s">
         <v>222</v>
@@ -3197,10 +3200,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="B132" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="C132" t="s">
         <v>222</v>
@@ -3211,10 +3214,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B133" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C133" t="s">
         <v>222</v>
@@ -3225,13 +3228,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B134" t="s">
-        <v>229</v>
+        <v>294</v>
       </c>
       <c r="C134" t="s">
-        <v>4</v>
+        <v>222</v>
       </c>
       <c r="D134" t="s">
         <v>169</v>
@@ -3239,13 +3242,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B135" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C135" t="s">
-        <v>32</v>
+        <v>166</v>
       </c>
       <c r="D135" t="s">
         <v>169</v>
@@ -3253,69 +3256,69 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>137</v>
+        <v>1</v>
       </c>
       <c r="B136" t="s">
-        <v>226</v>
+        <v>168</v>
       </c>
       <c r="C136" t="s">
         <v>166</v>
       </c>
       <c r="D136" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="B137" t="s">
-        <v>225</v>
+        <v>275</v>
       </c>
       <c r="C137" t="s">
         <v>166</v>
       </c>
       <c r="D137" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B138" t="s">
-        <v>223</v>
+        <v>277</v>
       </c>
       <c r="C138" t="s">
         <v>166</v>
       </c>
       <c r="D138" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>140</v>
+        <v>89</v>
       </c>
       <c r="B139" t="s">
-        <v>224</v>
+        <v>257</v>
       </c>
       <c r="C139" t="s">
         <v>166</v>
       </c>
       <c r="D139" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="B140" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="C140" t="s">
-        <v>220</v>
+        <v>166</v>
       </c>
       <c r="D140" t="s">
         <v>169</v>
@@ -3323,69 +3326,69 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="B141" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
       <c r="C141" t="s">
-        <v>222</v>
+        <v>166</v>
       </c>
       <c r="D141" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="B142" t="s">
-        <v>301</v>
+        <v>260</v>
       </c>
       <c r="C142" t="s">
-        <v>222</v>
+        <v>166</v>
       </c>
       <c r="D142" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="B143" t="s">
-        <v>305</v>
+        <v>276</v>
       </c>
       <c r="C143" t="s">
-        <v>221</v>
+        <v>166</v>
       </c>
       <c r="D143" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="B144" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
       <c r="C144" t="s">
-        <v>222</v>
+        <v>166</v>
       </c>
       <c r="D144" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B145" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C145" t="s">
-        <v>220</v>
+        <v>166</v>
       </c>
       <c r="D145" t="s">
         <v>169</v>
@@ -3393,125 +3396,125 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="B146" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
       <c r="C146" t="s">
-        <v>222</v>
+        <v>166</v>
       </c>
       <c r="D146" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>148</v>
+        <v>47</v>
       </c>
       <c r="B147" t="s">
-        <v>306</v>
+        <v>210</v>
       </c>
       <c r="C147" t="s">
-        <v>221</v>
+        <v>35</v>
       </c>
       <c r="D147" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>149</v>
+        <v>46</v>
       </c>
       <c r="B148" t="s">
-        <v>305</v>
+        <v>209</v>
       </c>
       <c r="C148" t="s">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="D148" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>150</v>
+        <v>48</v>
       </c>
       <c r="B149" t="s">
-        <v>306</v>
+        <v>195</v>
       </c>
       <c r="C149" t="s">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="D149" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>151</v>
+        <v>43</v>
       </c>
       <c r="B150" t="s">
-        <v>307</v>
+        <v>207</v>
       </c>
       <c r="C150" t="s">
-        <v>166</v>
+        <v>35</v>
       </c>
       <c r="D150" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>152</v>
+        <v>45</v>
       </c>
       <c r="B151" t="s">
-        <v>308</v>
+        <v>194</v>
       </c>
       <c r="C151" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D151" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>153</v>
+        <v>44</v>
       </c>
       <c r="B152" t="s">
-        <v>309</v>
+        <v>208</v>
       </c>
       <c r="C152" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D152" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>154</v>
+        <v>42</v>
       </c>
       <c r="B153" t="s">
-        <v>310</v>
+        <v>190</v>
       </c>
       <c r="C153" t="s">
-        <v>228</v>
+        <v>35</v>
       </c>
       <c r="D153" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="B154" t="s">
-        <v>311</v>
+        <v>290</v>
       </c>
       <c r="C154" t="s">
-        <v>12</v>
+        <v>220</v>
       </c>
       <c r="D154" t="s">
         <v>169</v>
@@ -3519,13 +3522,13 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="B155" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
       <c r="C155" t="s">
-        <v>166</v>
+        <v>220</v>
       </c>
       <c r="D155" t="s">
         <v>169</v>
@@ -3533,27 +3536,27 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="B156" t="s">
-        <v>313</v>
+        <v>164</v>
       </c>
       <c r="C156" t="s">
-        <v>227</v>
+        <v>166</v>
       </c>
       <c r="D156" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="B157" t="s">
-        <v>318</v>
+        <v>288</v>
       </c>
       <c r="C157" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D157" t="s">
         <v>169</v>
@@ -3561,13 +3564,13 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>159</v>
+        <v>120</v>
       </c>
       <c r="B158" t="s">
-        <v>316</v>
+        <v>282</v>
       </c>
       <c r="C158" t="s">
-        <v>12</v>
+        <v>220</v>
       </c>
       <c r="D158" t="s">
         <v>169</v>
@@ -3575,47 +3578,47 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>160</v>
+        <v>29</v>
       </c>
       <c r="B159" t="s">
-        <v>317</v>
+        <v>187</v>
       </c>
       <c r="C159" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D159" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>161</v>
+        <v>30</v>
       </c>
       <c r="B160" t="s">
-        <v>315</v>
+        <v>187</v>
       </c>
       <c r="C160" t="s">
         <v>12</v>
       </c>
       <c r="D160" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>162</v>
+        <v>13</v>
       </c>
       <c r="B161" t="s">
-        <v>314</v>
-      </c>
-      <c r="C161" t="s">
-        <v>12</v>
+        <v>182</v>
       </c>
       <c r="D161" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D161">
+    <sortCondition ref="A6:A161"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
arreglo indice metadata arg
</commit_message>
<xml_diff>
--- a/analisis/resultados/argentina/metadata_arg.xlsx
+++ b/analisis/resultados/argentina/metadata_arg.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos\repos\hidrocarburos\analisis\resultados\argentina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9310E781-F9E7-478A-BDE4-813BF88F7D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C4242C-DA1A-421C-A305-CEA21DC0A8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="indice" sheetId="2" r:id="rId1"/>
+    <sheet name="variables" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="369">
   <si>
     <t>variable</t>
   </si>
@@ -977,13 +978,163 @@
   </si>
   <si>
     <t>Costos totales hidrocarburíferos con ganancia normal</t>
+  </si>
+  <si>
+    <t>hoja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum_mecanismos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">descuentos_vbp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sobre_pib_mecanismos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">crudo_dif_precios </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gas_dif_precios </t>
+  </si>
+  <si>
+    <t xml:space="preserve">regalias </t>
+  </si>
+  <si>
+    <t xml:space="preserve">retenciones </t>
+  </si>
+  <si>
+    <t xml:space="preserve">subsidios </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tg_total </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tg_empresas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ccnn_oficial </t>
+  </si>
+  <si>
+    <t>criterio_ccnn</t>
+  </si>
+  <si>
+    <t>empalme_ccnn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criterio_propio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">comparacion_autores </t>
+  </si>
+  <si>
+    <t xml:space="preserve">segmento_YPF_PetBR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">costos_comparacion </t>
+  </si>
+  <si>
+    <t>Renta de la tierra del petróleo y el gas calculada como la suma de los mecanismos de apropiación por diferentes sujetos sociales</t>
+  </si>
+  <si>
+    <t>Renta de la tierra del petróleo y el gas calculada desde el producto de valor a precio internacional y valuda en moneda local por tipo de cambio de paridad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sobre_pib_descuentos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renta de la tierra hidrocarburífera estimada por suma de mecanismos sobre PBI y plusvalía total de la economia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renta de la tierra hidrocarburífera estimada desde descuento sobre producto a precio internacional sobre PBI y plusvalía total de la economia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">crudo_sobrevaluacion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gas_sobrevaluacion </t>
+  </si>
+  <si>
+    <t>costos_ccnn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stock_balances </t>
+  </si>
+  <si>
+    <t>tg_indu_jic</t>
+  </si>
+  <si>
+    <t>tg_indu_em</t>
+  </si>
+  <si>
+    <t>union_tg</t>
+  </si>
+  <si>
+    <t>renta_con_tg_jic</t>
+  </si>
+  <si>
+    <t>renta_con_tg_em</t>
+  </si>
+  <si>
+    <t>renta_con_tg_union</t>
+  </si>
+  <si>
+    <t>Mussi (2019)</t>
+  </si>
+  <si>
+    <t>Iñigo Carrera (2007) y Mussi (2019)</t>
+  </si>
+  <si>
+    <t>Tasa de ganancia del sector industrial</t>
+  </si>
+  <si>
+    <t>Renta de la tierra hidrocarburífera por diferencial de tasas de ganancia</t>
+  </si>
+  <si>
+    <t>stock_seleccionado</t>
+  </si>
+  <si>
+    <t>Stock de Propiedad, Planta y Equipo seleccionado</t>
+  </si>
+  <si>
+    <t>Tasa de ganancia total hidrocarburífera y renta de la tierra total apropiada por las empresas de la rama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasa de ganancia y renta de la tierra apropiada por cada empresa de la rama </t>
+  </si>
+  <si>
+    <t>Estimacion propia con criterio CCNN</t>
+  </si>
+  <si>
+    <t>Valores contables oficiales de las Cuentas Nacionales (CCNN)</t>
+  </si>
+  <si>
+    <t>Empalme entre valores contables oficiales de las CCNN y estimación propia con criterio CCNN</t>
+  </si>
+  <si>
+    <t>Valor del producto a precio exterior valuado en pesos por tcp</t>
+  </si>
+  <si>
+    <t>Estimaciones alternativas de renta de la tierra hidrocarburífera</t>
+  </si>
+  <si>
+    <t>Componentes del stock de empresas hidrocarburíferas</t>
+  </si>
+  <si>
+    <t>Información contable por segmento de YPF y Petrobras Argentina</t>
+  </si>
+  <si>
+    <t>Costos por barril de argentina, comparación con estimaciones alternativas</t>
+  </si>
+  <si>
+    <t>Costos por barril de argentina estimado a partir de CCNN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -998,6 +1149,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1020,11 +1175,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1362,11 +1518,214 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314A6900-C8B9-4455-83D4-0FFFBB16D0EC}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="130.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>324</v>
+      </c>
+      <c r="B7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>342</v>
+      </c>
+      <c r="B8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>343</v>
+      </c>
+      <c r="B9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>325</v>
+      </c>
+      <c r="B10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>326</v>
+      </c>
+      <c r="B11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>327</v>
+      </c>
+      <c r="B12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>328</v>
+      </c>
+      <c r="B13" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>329</v>
+      </c>
+      <c r="B14" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>345</v>
+      </c>
+      <c r="B15" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>335</v>
+      </c>
+      <c r="B16" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>330</v>
+      </c>
+      <c r="B17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>331</v>
+      </c>
+      <c r="B18" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>332</v>
+      </c>
+      <c r="B19" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>333</v>
+      </c>
+      <c r="B20" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>334</v>
+      </c>
+      <c r="B21" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>336</v>
+      </c>
+      <c r="B22" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>344</v>
+      </c>
+      <c r="B23" t="s">
+        <v>368</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D161"/>
+  <dimension ref="A1:H169"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView topLeftCell="A125" zoomScale="102" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,7 +1736,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3156,7 +3515,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>142</v>
       </c>
@@ -3170,7 +3529,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>143</v>
       </c>
@@ -3184,7 +3543,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>145</v>
       </c>
@@ -3198,7 +3557,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>147</v>
       </c>
@@ -3212,7 +3571,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>129</v>
       </c>
@@ -3225,8 +3584,9 @@
       <c r="D133" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H133" s="1"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>130</v>
       </c>
@@ -3239,139 +3599,133 @@
       <c r="D134" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H134" s="1"/>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B135" t="s">
-        <v>225</v>
+        <v>293</v>
       </c>
       <c r="C135" t="s">
-        <v>166</v>
+        <v>222</v>
       </c>
       <c r="D135" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H135" s="1"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>1</v>
+        <v>346</v>
       </c>
       <c r="B136" t="s">
-        <v>168</v>
+        <v>354</v>
       </c>
       <c r="C136" t="s">
-        <v>166</v>
+        <v>222</v>
       </c>
       <c r="D136" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="H136" s="1"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>111</v>
+        <v>347</v>
       </c>
       <c r="B137" t="s">
-        <v>275</v>
+        <v>354</v>
       </c>
       <c r="C137" t="s">
-        <v>166</v>
+        <v>222</v>
       </c>
       <c r="D137" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>113</v>
+        <v>348</v>
       </c>
       <c r="B138" t="s">
-        <v>277</v>
+        <v>354</v>
       </c>
       <c r="C138" t="s">
-        <v>166</v>
+        <v>222</v>
       </c>
       <c r="D138" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>89</v>
+        <v>349</v>
       </c>
       <c r="B139" t="s">
-        <v>257</v>
-      </c>
-      <c r="C139" t="s">
-        <v>166</v>
+        <v>355</v>
       </c>
       <c r="D139" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>156</v>
+        <v>350</v>
       </c>
       <c r="B140" t="s">
-        <v>312</v>
-      </c>
-      <c r="C140" t="s">
-        <v>166</v>
+        <v>355</v>
       </c>
       <c r="D140" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>99</v>
+        <v>351</v>
       </c>
       <c r="B141" t="s">
-        <v>265</v>
-      </c>
-      <c r="C141" t="s">
-        <v>166</v>
+        <v>355</v>
       </c>
       <c r="D141" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>92</v>
+        <v>356</v>
       </c>
       <c r="B142" t="s">
-        <v>260</v>
+        <v>357</v>
       </c>
       <c r="C142" t="s">
         <v>166</v>
       </c>
       <c r="D142" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="B143" t="s">
-        <v>276</v>
+        <v>225</v>
       </c>
       <c r="C143" t="s">
         <v>166</v>
       </c>
       <c r="D143" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>114</v>
+        <v>1</v>
       </c>
       <c r="B144" t="s">
-        <v>278</v>
+        <v>168</v>
       </c>
       <c r="C144" t="s">
         <v>166</v>
@@ -3382,24 +3736,24 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="B145" t="s">
-        <v>307</v>
+        <v>275</v>
       </c>
       <c r="C145" t="s">
         <v>166</v>
       </c>
       <c r="D145" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="B146" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="C146" t="s">
         <v>166</v>
@@ -3410,181 +3764,181 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="B147" t="s">
-        <v>210</v>
+        <v>257</v>
       </c>
       <c r="C147" t="s">
-        <v>35</v>
+        <v>166</v>
       </c>
       <c r="D147" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>46</v>
+        <v>156</v>
       </c>
       <c r="B148" t="s">
-        <v>209</v>
+        <v>312</v>
       </c>
       <c r="C148" t="s">
-        <v>35</v>
+        <v>166</v>
       </c>
       <c r="D148" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="B149" t="s">
-        <v>195</v>
+        <v>265</v>
       </c>
       <c r="C149" t="s">
-        <v>35</v>
+        <v>166</v>
       </c>
       <c r="D149" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="B150" t="s">
-        <v>207</v>
+        <v>260</v>
       </c>
       <c r="C150" t="s">
-        <v>35</v>
+        <v>166</v>
       </c>
       <c r="D150" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="B151" t="s">
-        <v>194</v>
+        <v>276</v>
       </c>
       <c r="C151" t="s">
-        <v>35</v>
+        <v>166</v>
       </c>
       <c r="D151" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="B152" t="s">
-        <v>208</v>
+        <v>278</v>
       </c>
       <c r="C152" t="s">
-        <v>35</v>
+        <v>166</v>
       </c>
       <c r="D152" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>42</v>
+        <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>190</v>
+        <v>307</v>
       </c>
       <c r="C153" t="s">
-        <v>35</v>
+        <v>166</v>
       </c>
       <c r="D153" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="B154" t="s">
-        <v>290</v>
+        <v>263</v>
       </c>
       <c r="C154" t="s">
-        <v>220</v>
+        <v>166</v>
       </c>
       <c r="D154" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>121</v>
+        <v>47</v>
       </c>
       <c r="B155" t="s">
-        <v>283</v>
+        <v>210</v>
       </c>
       <c r="C155" t="s">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="D155" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B156" t="s">
-        <v>164</v>
+        <v>209</v>
       </c>
       <c r="C156" t="s">
-        <v>166</v>
+        <v>35</v>
       </c>
       <c r="D156" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
       <c r="B157" t="s">
-        <v>288</v>
+        <v>195</v>
       </c>
       <c r="C157" t="s">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="D157" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>120</v>
+        <v>43</v>
       </c>
       <c r="B158" t="s">
-        <v>282</v>
+        <v>207</v>
       </c>
       <c r="C158" t="s">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="D158" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B159" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="C159" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D159" t="s">
         <v>175</v>
@@ -3592,32 +3946,144 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B160" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
       <c r="C160" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D160" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
+        <v>42</v>
+      </c>
+      <c r="B161" t="s">
+        <v>190</v>
+      </c>
+      <c r="C161" t="s">
+        <v>35</v>
+      </c>
+      <c r="D161" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>126</v>
+      </c>
+      <c r="B162" t="s">
+        <v>290</v>
+      </c>
+      <c r="C162" t="s">
+        <v>220</v>
+      </c>
+      <c r="D162" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>121</v>
+      </c>
+      <c r="B163" t="s">
+        <v>283</v>
+      </c>
+      <c r="C163" t="s">
+        <v>220</v>
+      </c>
+      <c r="D163" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>0</v>
+      </c>
+      <c r="B164" t="s">
+        <v>164</v>
+      </c>
+      <c r="C164" t="s">
+        <v>166</v>
+      </c>
+      <c r="D164" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>124</v>
+      </c>
+      <c r="B165" t="s">
+        <v>288</v>
+      </c>
+      <c r="C165" t="s">
+        <v>220</v>
+      </c>
+      <c r="D165" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>120</v>
+      </c>
+      <c r="B166" t="s">
+        <v>282</v>
+      </c>
+      <c r="C166" t="s">
+        <v>220</v>
+      </c>
+      <c r="D166" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>29</v>
+      </c>
+      <c r="B167" t="s">
+        <v>187</v>
+      </c>
+      <c r="C167" t="s">
+        <v>12</v>
+      </c>
+      <c r="D167" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>30</v>
+      </c>
+      <c r="B168" t="s">
+        <v>187</v>
+      </c>
+      <c r="C168" t="s">
+        <v>12</v>
+      </c>
+      <c r="D168" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>13</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B169" t="s">
         <v>182</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D169" t="s">
         <v>176</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D161">
-    <sortCondition ref="A6:A161"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D169">
+    <sortCondition ref="A6:A169"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
termino primer limpieza de visualizacion ganancia
</commit_message>
<xml_diff>
--- a/analisis/resultados/argentina/metadata_arg.xlsx
+++ b/analisis/resultados/argentina/metadata_arg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos\repos\pioYPFConicet\analisis\resultados\argentina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AF606E-D829-43CC-BE52-B5A44478BDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF30450-F651-4076-849E-F31ED151798B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indice" sheetId="2" r:id="rId1"/>
@@ -89,12 +89,6 @@
     <t>hoja</t>
   </si>
   <si>
-    <t xml:space="preserve">gas_dif_precios </t>
-  </si>
-  <si>
-    <t xml:space="preserve">segmento_YPF_PetBR </t>
-  </si>
-  <si>
     <t>Renta de la tierra del petróleo y el gas calculada como la suma de los mecanismos de apropiación por diferentes sujetos sociales</t>
   </si>
   <si>
@@ -687,6 +681,12 @@
   </si>
   <si>
     <t>RTPG_PextQ</t>
+  </si>
+  <si>
+    <t>gas_dif_precios _y_sv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">segmentos_YPF_PetBR </t>
   </si>
 </sst>
 </file>
@@ -1070,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314A6900-C8B9-4455-83D4-0FFFBB16D0EC}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,178 +1092,178 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>220</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>220</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>43</v>
+      <c r="A14" t="s">
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>45</v>
+      <c r="A17" s="2" t="s">
+        <v>221</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>51</v>
+      <c r="A23" t="s">
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1307,71 +1307,71 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -1379,63 +1379,63 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -1443,18 +1443,18 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1467,15 +1467,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
         <v>17</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B26" t="s">
         <v>18</v>
@@ -1491,159 +1491,159 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B31" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B35" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B38" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B39" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B41" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B42" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B43" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B44" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B46" t="s">
         <v>20</v>
@@ -1651,23 +1651,23 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B47" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B49" t="s">
         <v>19</v>
@@ -1675,87 +1675,87 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B50" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B51" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B52" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B53" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B56" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B57" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B58" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B59" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B60" t="s">
         <v>15</v>
@@ -1763,103 +1763,103 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B61" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B62" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B63" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B64" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B65" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B66" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B67" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B68" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B69" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B70" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B71" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B72" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B73" t="s">
         <v>12</v>
@@ -1867,47 +1867,47 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B75" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B76" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B77" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B78" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B79" t="s">
         <v>11</v>
@@ -1915,15 +1915,15 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B80" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B81" t="s">
         <v>13</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B82" t="s">
         <v>9</v>
@@ -1942,39 +1942,39 @@
         <v>1</v>
       </c>
       <c r="B83" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B84" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B85" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B86" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B87" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1987,10 +1987,10 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B89" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>